<commit_message>
Table 4 done marine
</commit_message>
<xml_diff>
--- a/Table4_Marine.xlsx
+++ b/Table4_Marine.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -26,22 +26,28 @@
     <t xml:space="preserve">Natura 2000 i alt</t>
   </si>
   <si>
-    <t xml:space="preserve">Kun habitatomräde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kun Habitatnaturtype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kun ramsar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kun Havstrategi standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kun Havstrategi streng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kun Natur Vildt Reservater</t>
+    <t xml:space="preserve">Kun fuglebeskyt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun habitatomraade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitatatomr. og fuglebesk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitatnaturtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramsar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Havstrategi standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Havstrategi streng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vildt Reservater</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>30478.8135</v>
+        <v>26284.8191</v>
       </c>
       <c r="C2" t="n">
-        <v>29.0217462514941</v>
+        <v>25.0282495473987</v>
       </c>
     </row>
     <row r="3">
@@ -400,10 +406,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>19979.975</v>
+        <v>22270.9031</v>
       </c>
       <c r="C3" t="n">
-        <v>19.0248142225482</v>
+        <v>21.2062224325042</v>
       </c>
     </row>
     <row r="4">
@@ -411,10 +417,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>7589.0613</v>
+        <v>16074.5452</v>
       </c>
       <c r="C4" t="n">
-        <v>7.2262593599857</v>
+        <v>15.3060870267332</v>
       </c>
     </row>
     <row r="5">
@@ -422,10 +428,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>7279.4093</v>
+        <v>12060.63</v>
       </c>
       <c r="C5" t="n">
-        <v>6.93141055393662</v>
+        <v>11.484060673594</v>
       </c>
     </row>
     <row r="6">
@@ -433,10 +439,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>3495.7145</v>
+        <v>7105.5811</v>
       </c>
       <c r="C6" t="n">
-        <v>3.32859870633312</v>
+        <v>6.76589236827123</v>
       </c>
     </row>
     <row r="7">
@@ -444,10 +450,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>3281.2006</v>
+        <v>5647.0395</v>
       </c>
       <c r="C7" t="n">
-        <v>3.12433983735784</v>
+        <v>5.37707766876043</v>
       </c>
     </row>
     <row r="8">
@@ -455,10 +461,32 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>3170.2273</v>
+        <v>3494.8231</v>
       </c>
       <c r="C8" t="n">
-        <v>3.01867171634352</v>
+        <v>3.32774992051642</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3280.8196</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.12397705140747</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2290.1955</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.18071063256165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>